<commit_message>
aangepast nav Marcels commentaar
</commit_message>
<xml_diff>
--- a/data/deltares/intern/raakvlakken.xlsx
+++ b/data/deltares/intern/raakvlakken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_checkouts\zeespiegelmonitor2022\data\deltares\intern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776CCAED-1585-4E92-82BC-81E91D6500F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625AE499-05AF-4FAA-9E8E-B8F7A5CC4FC1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="972" yWindow="-108" windowWidth="22176" windowHeight="13176" activeTab="2" xr2:uid="{3B55AA0C-0BCC-4C0D-A055-47F3A622DE26}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
   <si>
     <t>Deltares</t>
   </si>
@@ -137,9 +137,6 @@
     <t>programma</t>
   </si>
   <si>
-    <t>extremen zeespiegel en golven</t>
-  </si>
-  <si>
     <t>extremen zeespiegel</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>https://www.rijkswaterstaat.nl/water/waterbeheer/metingen/meten-bij-rijkswaterstaat/waternormalen#:~:text=Rijkswaterstaat%20verzamelt%20al%20jaren%20gegevens,we%20enkele%20tientallen%20jaren%20lang.</t>
   </si>
   <si>
-    <t>zeespiegel(stijging), bodemdaling</t>
-  </si>
-  <si>
     <t>opdrachtgever</t>
   </si>
   <si>
@@ -219,6 +213,33 @@
   </si>
   <si>
     <t>https://puc.overheid.nl/rijkswaterstaat/doc/PUC_695110_31/1/)</t>
+  </si>
+  <si>
+    <t>KP ZSS Spoor I Zeespiegelstijging en Antarctica</t>
+  </si>
+  <si>
+    <t>KP ZSS Spoor II Systeemverkenningen</t>
+  </si>
+  <si>
+    <t>KP ZSS Spoor V Implementatiestrategie</t>
+  </si>
+  <si>
+    <t>KP ZSS Spoor IV Langetermijnopties</t>
+  </si>
+  <si>
+    <t>KP ZSS Spoor III Signaleringsmethodiek</t>
+  </si>
+  <si>
+    <t>Programma Beoordelings- en 
+Ontwerpinstrumentarium (BOI 2023)</t>
+  </si>
+  <si>
+    <t>zeespiegel(stijging), 
+bodemdaling</t>
+  </si>
+  <si>
+    <t>extremen zeespiegel,
+golven</t>
   </si>
 </sst>
 </file>
@@ -263,10 +284,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -596,7 +623,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -607,15 +634,15 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -623,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -631,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -639,23 +666,23 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -694,7 +721,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -706,16 +733,16 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -723,10 +750,10 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -734,10 +761,10 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -745,10 +772,10 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -756,10 +783,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -792,7 +819,7 @@
         <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -800,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -824,7 +851,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,10 +868,10 @@
         <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>32</v>
@@ -858,7 +885,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -867,29 +894,29 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
+        <v>35</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>56</v>
+        <v>35</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -908,13 +935,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -922,7 +949,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -933,13 +960,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -947,7 +974,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -958,7 +985,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -969,7 +996,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
@@ -981,15 +1008,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
@@ -1000,10 +1027,10 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -1014,7 +1041,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
@@ -1025,30 +1052,30 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>